<commit_message>
Ej. 2a. ley Newton - 9 de enero de 2024 - Lap HP
Se hace actualización del repositorio hasta los ejercicios en clase del día 9 de enero de 2024.
</commit_message>
<xml_diff>
--- a/Bitacoras/NRC_124_Grupo_43/Bitacora_Evaluacion_Continua_Parcial_02_NRC_124.xlsx
+++ b/Bitacoras/NRC_124_Grupo_43/Bitacora_Evaluacion_Continua_Parcial_02_NRC_124.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_124_Grupo_43\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5505158-E67D-4E18-9B4D-09D5EF82E51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFD9455-EDD0-4EDF-A69F-9992A79FD403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{3B38BCB7-8149-4E80-B00A-D09192B22F60}"/>
   </bookViews>
@@ -902,10 +902,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8032F5A0-642F-4560-B0C5-3C9690CB9299}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,30 +995,30 @@
         <v>8</v>
       </c>
       <c r="F3" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G3" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H3" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I3" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J3" s="2">
         <v>0</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" ref="K3:K31" si="0">SUM(F3:J3)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L3" s="3">
         <f>(K3/23)*10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>7.8260869565217392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20244739</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>9.5652173913043477</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10186663</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10187045</v>
       </c>
@@ -1137,7 +1138,7 @@
         <v>6.5217391304347831</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10186376</v>
       </c>
@@ -1177,7 +1178,7 @@
         <v>7.391304347826086</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20238395</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>9.913043478260871</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10185692</v>
       </c>
@@ -1257,7 +1258,7 @@
         <v>6.9565217391304346</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20266322</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20245456</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10186574</v>
       </c>
@@ -1377,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20249032</v>
       </c>
@@ -1417,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>20266998</v>
       </c>
@@ -1457,7 +1458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20264862</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20268353</v>
       </c>
@@ -1537,7 +1538,7 @@
         <v>1.3043478260869565</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20264649</v>
       </c>
@@ -1577,7 +1578,7 @@
         <v>1.7391304347826086</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10187502</v>
       </c>
@@ -1617,7 +1618,7 @@
         <v>9.7391304347826075</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>20235464</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>0.43478260869565216</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20247651</v>
       </c>
@@ -1697,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20244756</v>
       </c>
@@ -1737,7 +1738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20266315</v>
       </c>
@@ -1777,7 +1778,7 @@
         <v>8.2608695652173907</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20271313</v>
       </c>
@@ -1817,7 +1818,7 @@
         <v>5.108695652173914</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20266724</v>
       </c>
@@ -1857,7 +1858,7 @@
         <v>2.8260869565217388</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20251515</v>
       </c>
@@ -1897,7 +1898,7 @@
         <v>9.4347826086956523</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20250030</v>
       </c>
@@ -1937,7 +1938,7 @@
         <v>9.5652173913043477</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20266265</v>
       </c>
@@ -1977,7 +1978,7 @@
         <v>4.3478260869565215</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>20251561</v>
       </c>
@@ -2017,7 +2018,7 @@
         <v>3.0434782608695654</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>10186004</v>
       </c>
@@ -2057,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20270002</v>
       </c>
@@ -2097,7 +2098,7 @@
         <v>9.8478260869565215</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10186676</v>
       </c>
@@ -2138,7 +2139,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:L31" xr:uid="{8032F5A0-642F-4560-B0C5-3C9690CB9299}"/>
+  <autoFilter ref="A2:L31" xr:uid="{8032F5A0-642F-4560-B0C5-3C9690CB9299}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="ANDRADE DELGADO BRYANA"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:L31">
     <sortCondition ref="B3:B31"/>
   </sortState>
@@ -5992,8 +5999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12306488-44B1-431C-AA6F-378310B077F5}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6033,14 +6040,14 @@
         <v>5</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>7.83</v>
       </c>
       <c r="D2" s="3">
         <v>8.65</v>
       </c>
       <c r="E2" s="3">
         <f>C2*0.4+D2*0.6</f>
-        <v>5.19</v>
+        <v>8.322000000000001</v>
       </c>
       <c r="F2" s="4">
         <v>6</v>

</xml_diff>